<commit_message>
saving changes to local
</commit_message>
<xml_diff>
--- a/SkillArcade-QuizDataSet.xlsx
+++ b/SkillArcade-QuizDataSet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navya\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\project-se\SkillArcade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16E93ED-AF68-40CB-A992-8C06BAD6B41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D027A341-AF29-4663-AEE9-57B5EC366661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{36D17A26-940A-4B6A-AE2E-8CCDFD8B8B5D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{36D17A26-940A-4B6A-AE2E-8CCDFD8B8B5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Technology" sheetId="1" r:id="rId1"/>
@@ -21,21 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="114">
   <si>
     <t>Category</t>
   </si>
@@ -394,6 +385,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>h</t>
   </si>
 </sst>
 </file>
@@ -477,13 +471,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -825,11 +818,11 @@
       <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1331,7 +1324,7 @@
       <c r="A46" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" t="s">
         <v>72</v>
       </c>
       <c r="C46" t="s">
@@ -1342,7 +1335,7 @@
       <c r="A47" t="s">
         <v>68</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" t="s">
         <v>72</v>
       </c>
       <c r="C47" t="s">
@@ -1353,7 +1346,7 @@
       <c r="A48" t="s">
         <v>75</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" t="s">
         <v>76</v>
       </c>
       <c r="C48" t="s">
@@ -1364,7 +1357,7 @@
       <c r="A49" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" t="s">
         <v>76</v>
       </c>
       <c r="C49" t="s">
@@ -1400,376 +1393,381 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B3EDC5-55D0-48D7-8418-CCDDD12B9F62}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="12"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="8.90625" style="11"/>
+    <col min="2" max="2" width="37.90625" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8">
-      <c r="A2" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:5" ht="29">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="10">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8">
-      <c r="A3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:5" ht="29">
+      <c r="A3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="10">
         <v>2</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>67</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8">
-      <c r="A4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:5" ht="29">
+      <c r="A4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="10">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
-      <c r="A5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="1:5" ht="29">
+      <c r="A5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8">
-      <c r="A6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="1:5" ht="43.5">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="11">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28.8">
-      <c r="A7" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:5" ht="43.5">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C7" s="10">
         <v>2</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
-      <c r="A8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="1:5" ht="43.5">
+      <c r="A8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="10">
         <v>3</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="28.8">
-      <c r="A9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="1:5" ht="43.5">
+      <c r="A9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="10">
         <v>4</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>1</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="10">
         <v>2</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="10">
         <v>3</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="10">
         <v>4</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8">
-      <c r="A14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="6" t="s">
+    <row r="14" spans="1:5" ht="29">
+      <c r="A14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <v>1</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8">
-      <c r="A15" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="1:5" ht="29">
+      <c r="A15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <v>2</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.2">
-      <c r="A16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:5" ht="43.5">
+      <c r="A16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>3</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="28.8">
-      <c r="A17" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="6" t="s">
+    <row r="17" spans="1:5" ht="29">
+      <c r="A17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>4</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8">
-      <c r="A18" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="6" t="s">
+    <row r="18" spans="1:5" ht="29">
+      <c r="A18" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>1</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="28.8">
-      <c r="A19" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="1:5" ht="29">
+      <c r="A19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="10">
         <v>2</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="28.8">
-      <c r="A20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="1:5" ht="29">
+      <c r="A20" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>3</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8">
-      <c r="A21" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="1:5" ht="29">
+      <c r="A21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C21" s="10">
         <v>4</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="11" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>